<commit_message>
Fixed some typos, re-arraged examples
</commit_message>
<xml_diff>
--- a/docs/Examples/Calc4.xlsx
+++ b/docs/Examples/Calc4.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
   <si>
     <t>P_kbar_calc</t>
   </si>
@@ -245,6 +245,15 @@
   </si>
   <si>
     <t>Al_VI_cat_6ox</t>
+  </si>
+  <si>
+    <t>En_Simple_MgFeCa_Cpx</t>
+  </si>
+  <si>
+    <t>Fs_Simple_MgFeCa_Cpx</t>
+  </si>
+  <si>
+    <t>Wo_Simple_MgFeCa_Cpx</t>
   </si>
   <si>
     <t>Cation_Sum_Cpx</t>
@@ -752,13 +761,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:DX6"/>
+  <dimension ref="A1:EA6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:128">
+    <row r="1" spans="1:131">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1140,8 +1149,17 @@
       <c r="DX1" s="1" t="s">
         <v>126</v>
       </c>
+      <c r="DY1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="DZ1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="EA1" s="1" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="2" spans="1:128">
+    <row r="2" spans="1:131">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1377,157 +1395,166 @@
         <v>0.04743015771494319</v>
       </c>
       <c r="CA2">
+        <v>0.4502338274974608</v>
+      </c>
+      <c r="CB2">
+        <v>0.08280532061471052</v>
+      </c>
+      <c r="CC2">
+        <v>0.4669608518878287</v>
+      </c>
+      <c r="CD2">
         <v>4.017665755622844</v>
       </c>
-      <c r="CB2">
+      <c r="CE2">
         <v>0.4669608518878287</v>
       </c>
-      <c r="CC2">
+      <c r="CF2">
         <v>0.03533151124568563</v>
       </c>
-      <c r="CD2">
+      <c r="CG2">
         <v>0.1234457426604853</v>
       </c>
-      <c r="CE2">
+      <c r="CH2">
         <v>0.2225224985095453</v>
       </c>
-      <c r="CF2">
+      <c r="CI2">
         <v>0.009562446737175665</v>
       </c>
-      <c r="CG2">
+      <c r="CJ2">
         <v>0.0789769949359318</v>
       </c>
-      <c r="CH2">
+      <c r="CK2">
         <v>0.8446499523459867</v>
       </c>
-      <c r="CI2">
+      <c r="CL2">
         <v>0.01705536082466275</v>
       </c>
-      <c r="CJ2">
-        <v>0</v>
-      </c>
-      <c r="CK2">
+      <c r="CM2">
+        <v>0</v>
+      </c>
+      <c r="CN2">
         <v>0.03037479689028044</v>
       </c>
-      <c r="CL2">
+      <c r="CO2">
         <v>0.04101305128916294</v>
       </c>
-      <c r="CM2">
+      <c r="CP2">
         <v>0.8144361511961696</v>
       </c>
-      <c r="CN2">
+      <c r="CQ2">
         <v>0.1038269365668692</v>
       </c>
-      <c r="CO2">
+      <c r="CR2">
         <v>0.8144361511961696</v>
       </c>
-      <c r="CP2">
+      <c r="CS2">
         <v>0.6860416366178594</v>
       </c>
-      <c r="CQ2">
+      <c r="CT2">
         <v>0.03533151124568563</v>
       </c>
-      <c r="CR2">
+      <c r="CU2">
         <v>0.1234457426604853</v>
       </c>
-      <c r="CS2">
+      <c r="CV2">
         <v>0.2240847291480202</v>
       </c>
-      <c r="CT2">
+      <c r="CW2">
         <v>0.174220835340168</v>
       </c>
-      <c r="CU2">
+      <c r="CX2">
         <v>0.2240847291480202</v>
       </c>
-      <c r="CV2">
+      <c r="CY2">
         <v>1.862542008564363</v>
       </c>
-      <c r="CW2">
+      <c r="CZ2">
         <v>-3.499393232656884</v>
       </c>
-      <c r="CX2">
+      <c r="DA2">
         <v>-3.499393232656884</v>
       </c>
-      <c r="CY2">
+      <c r="DB2">
         <v>0.2661048911363535</v>
       </c>
-      <c r="CZ2">
+      <c r="DC2">
         <v>0.5492176786163681</v>
       </c>
-      <c r="DA2">
+      <c r="DD2">
         <v>0.5492176786163681</v>
       </c>
-      <c r="DB2">
+      <c r="DE2">
         <v>0.0420201619883333</v>
       </c>
-      <c r="DC2">
+      <c r="DF2">
         <v>0.2549709601722976</v>
       </c>
-      <c r="DD2">
+      <c r="DG2">
         <v>0.1199035275390813</v>
       </c>
-      <c r="DE2">
+      <c r="DH2">
         <v>0.0308862310242774</v>
       </c>
-      <c r="DF2">
+      <c r="DI2">
         <v>0.9387708135379146</v>
       </c>
-      <c r="DG2">
+      <c r="DJ2">
         <v>0.124334662341745</v>
       </c>
-      <c r="DH2">
+      <c r="DK2">
         <v>0.7102334021213806</v>
       </c>
-      <c r="DI2">
+      <c r="DL2">
         <v>0.104202749074789</v>
       </c>
-      <c r="DJ2">
+      <c r="DM2">
         <v>0.7641722680523966</v>
       </c>
-      <c r="DK2">
+      <c r="DN2">
         <v>-0.05026388314377306</v>
       </c>
-      <c r="DL2">
+      <c r="DO2">
         <v>0.09176213088706986</v>
       </c>
-      <c r="DM2">
+      <c r="DP2">
         <v>-0.01206480567979934</v>
       </c>
-      <c r="DN2">
+      <c r="DQ2">
         <v>0.08649631336912542</v>
       </c>
-      <c r="DO2">
+      <c r="DR2">
         <v>-0.01733062319774378</v>
       </c>
-      <c r="DP2">
+      <c r="DS2">
         <v>0.01243809327092849</v>
       </c>
-      <c r="DQ2">
+      <c r="DT2">
         <v>-0.01793670361935194</v>
       </c>
-      <c r="DR2">
-        <v>0</v>
-      </c>
-      <c r="DS2">
+      <c r="DU2">
+        <v>0</v>
+      </c>
+      <c r="DV2">
         <v>0.009562446737175665</v>
       </c>
-      <c r="DT2">
+      <c r="DW2">
         <v>0.04490751495311449</v>
       </c>
-      <c r="DU2">
+      <c r="DX2">
         <v>0.003894463663951547</v>
       </c>
-      <c r="DV2">
+      <c r="DY2">
         <v>0.01618424696702273</v>
       </c>
-      <c r="DW2">
+      <c r="DZ2">
         <v>0.0008711138576400212</v>
       </c>
-      <c r="DX2">
+      <c r="EA2">
         <v>0.0008711138576400212</v>
       </c>
     </row>
-    <row r="3" spans="1:128">
+    <row r="3" spans="1:131">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1763,157 +1790,166 @@
         <v>0.05414697706282878</v>
       </c>
       <c r="CA3">
+        <v>0.4337060055370763</v>
+      </c>
+      <c r="CB3">
+        <v>0.09456276883405393</v>
+      </c>
+      <c r="CC3">
+        <v>0.4717312256288699</v>
+      </c>
+      <c r="CD3">
         <v>4.02036602591458</v>
       </c>
-      <c r="CB3">
+      <c r="CE3">
         <v>0.4717312256288699</v>
       </c>
-      <c r="CC3">
+      <c r="CF3">
         <v>0.04073205182916154</v>
       </c>
-      <c r="CD3">
+      <c r="CG3">
         <v>0.1408468819657791</v>
       </c>
-      <c r="CE3">
+      <c r="CH3">
         <v>0.2243214616248422</v>
       </c>
-      <c r="CF3">
+      <c r="CI3">
         <v>0.004122128302039983</v>
       </c>
-      <c r="CG3">
+      <c r="CJ3">
         <v>0.06892223540090255</v>
       </c>
-      <c r="CH3">
+      <c r="CK3">
         <v>0.8209900587021833</v>
       </c>
-      <c r="CI3">
+      <c r="CL3">
         <v>0.01733002910195383</v>
       </c>
-      <c r="CJ3">
-        <v>0</v>
-      </c>
-      <c r="CK3">
+      <c r="CM3">
+        <v>0</v>
+      </c>
+      <c r="CN3">
         <v>0.03681694796087495</v>
       </c>
-      <c r="CL3">
+      <c r="CO3">
         <v>0.04493815113685524</v>
       </c>
-      <c r="CM3">
+      <c r="CP3">
         <v>0.8199386031179183</v>
       </c>
-      <c r="CN3">
+      <c r="CQ3">
         <v>0.09722016629493835</v>
       </c>
-      <c r="CO3">
+      <c r="CR3">
         <v>0.8199386031179183</v>
       </c>
-      <c r="CP3">
+      <c r="CS3">
         <v>0.6731654672704361</v>
       </c>
-      <c r="CQ3">
+      <c r="CT3">
         <v>0.04073205182916154</v>
       </c>
-      <c r="CR3">
+      <c r="CU3">
         <v>0.1408468819657791</v>
       </c>
-      <c r="CS3">
+      <c r="CV3">
         <v>0.2224781609195403</v>
       </c>
-      <c r="CT3">
+      <c r="CW3">
         <v>0.1725715346824622</v>
       </c>
-      <c r="CU3">
+      <c r="CX3">
         <v>0.2224781609195403</v>
       </c>
-      <c r="CV3">
+      <c r="CY3">
         <v>1.712220738635643</v>
       </c>
-      <c r="CW3">
+      <c r="CZ3">
         <v>-3.892401433108129</v>
       </c>
-      <c r="CX3">
+      <c r="DA3">
         <v>-3.892401433108129</v>
       </c>
-      <c r="CY3">
+      <c r="DB3">
         <v>0.2617041509186061</v>
       </c>
-      <c r="CZ3">
+      <c r="DC3">
         <v>0.505035660474677</v>
       </c>
-      <c r="DA3">
+      <c r="DD3">
         <v>0.505035660474677</v>
       </c>
-      <c r="DB3">
+      <c r="DE3">
         <v>0.03922598999906582</v>
       </c>
-      <c r="DC3">
+      <c r="DF3">
         <v>0.2406315301949661</v>
       </c>
-      <c r="DD3">
+      <c r="DG3">
         <v>0.1153414798795298</v>
       </c>
-      <c r="DE3">
+      <c r="DH3">
         <v>0.01815336927542577</v>
       </c>
-      <c r="DF3">
+      <c r="DI3">
         <v>1.08713755714105</v>
       </c>
-      <c r="DG3">
+      <c r="DJ3">
         <v>0.2671989540231312</v>
       </c>
-      <c r="DH3">
+      <c r="DK3">
         <v>0.7093732963858266</v>
       </c>
-      <c r="DI3">
+      <c r="DL3">
         <v>0.1105653067320918</v>
       </c>
-      <c r="DJ3">
+      <c r="DM3">
         <v>0.7799637567469191</v>
       </c>
-      <c r="DK3">
+      <c r="DN3">
         <v>-0.03997484637099924</v>
       </c>
-      <c r="DL3">
+      <c r="DO3">
         <v>0.09067250557756676</v>
       </c>
-      <c r="DM3">
+      <c r="DP3">
         <v>-0.00654766071737159</v>
       </c>
-      <c r="DN3">
+      <c r="DQ3">
         <v>0.07957186151623884</v>
       </c>
-      <c r="DO3">
+      <c r="DR3">
         <v>-0.01764830477869951</v>
       </c>
-      <c r="DP3">
+      <c r="DS3">
         <v>0.01148615299423432</v>
       </c>
-      <c r="DQ3">
+      <c r="DT3">
         <v>-0.02533079496664063</v>
       </c>
-      <c r="DR3">
-        <v>0</v>
-      </c>
-      <c r="DS3">
+      <c r="DU3">
+        <v>0</v>
+      </c>
+      <c r="DV3">
         <v>0.004122128302039983</v>
       </c>
-      <c r="DT3">
+      <c r="DW3">
         <v>0.06042374229777</v>
       </c>
-      <c r="DU3">
+      <c r="DX3">
         <v>0.01548559116091475</v>
       </c>
-      <c r="DV3">
+      <c r="DY3">
         <v>0.01743017959050632</v>
       </c>
-      <c r="DW3">
+      <c r="DZ3">
         <v>0.0001001504885524938</v>
       </c>
-      <c r="DX3">
+      <c r="EA3">
         <v>0.0001001504885524938</v>
       </c>
     </row>
-    <row r="4" spans="1:128">
+    <row r="4" spans="1:131">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2149,157 +2185,166 @@
         <v>0.1099695945165395</v>
       </c>
       <c r="CA4">
+        <v>0.3978937584936887</v>
+      </c>
+      <c r="CB4">
+        <v>0.1109236796885445</v>
+      </c>
+      <c r="CC4">
+        <v>0.4911825618177668</v>
+      </c>
+      <c r="CD4">
         <v>4.019309316174092</v>
       </c>
-      <c r="CB4">
+      <c r="CE4">
         <v>0.4911825618177668</v>
       </c>
-      <c r="CC4">
+      <c r="CF4">
         <v>0.03861863234818354</v>
       </c>
-      <c r="CD4">
+      <c r="CG4">
         <v>0.1645079174277526</v>
       </c>
-      <c r="CE4">
+      <c r="CH4">
         <v>0.1901210471540171</v>
       </c>
-      <c r="CF4">
+      <c r="CI4">
         <v>0.003244703005003044</v>
       </c>
-      <c r="CG4">
+      <c r="CJ4">
         <v>0.06720473610028577</v>
       </c>
-      <c r="CH4">
+      <c r="CK4">
         <v>0.7819914000159349</v>
       </c>
-      <c r="CI4">
+      <c r="CL4">
         <v>0.01808493096752772</v>
       </c>
-      <c r="CJ4">
-        <v>0</v>
-      </c>
-      <c r="CK4">
+      <c r="CM4">
+        <v>0</v>
+      </c>
+      <c r="CN4">
         <v>0.09188466354901176</v>
       </c>
-      <c r="CL4">
+      <c r="CO4">
         <v>0.07166710610330454</v>
       </c>
-      <c r="CM4">
+      <c r="CP4">
         <v>0.7326707950378427</v>
       </c>
-      <c r="CN4">
+      <c r="CQ4">
         <v>0.09954497614876506</v>
       </c>
-      <c r="CO4">
+      <c r="CR4">
         <v>0.7326707950378427</v>
       </c>
-      <c r="CP4">
+      <c r="CS4">
         <v>0.5702387665641799</v>
       </c>
-      <c r="CQ4">
+      <c r="CT4">
         <v>0.03861863234818354</v>
       </c>
-      <c r="CR4">
+      <c r="CU4">
         <v>0.1645079174277526</v>
       </c>
-      <c r="CS4">
+      <c r="CV4">
         <v>0.3094015969114679</v>
       </c>
-      <c r="CT4">
+      <c r="CW4">
         <v>0.2505778413155346</v>
       </c>
-      <c r="CU4">
+      <c r="CX4">
         <v>0.3094015969114679</v>
       </c>
-      <c r="CV4">
+      <c r="CY4">
         <v>1.413884228092731</v>
       </c>
-      <c r="CW4">
+      <c r="CZ4">
         <v>-4.566443834840332</v>
       </c>
-      <c r="CX4">
+      <c r="DA4">
         <v>-4.566443834840332</v>
       </c>
-      <c r="CY4">
+      <c r="DB4">
         <v>0.2544504004029639</v>
       </c>
-      <c r="CZ4">
+      <c r="DC4">
         <v>0.526024972476467</v>
       </c>
-      <c r="DA4">
+      <c r="DD4">
         <v>0.526024972476467</v>
       </c>
-      <c r="DB4">
+      <c r="DE4">
         <v>0.054951196508504</v>
       </c>
-      <c r="DC4">
+      <c r="DF4">
         <v>0.2327166839143239</v>
       </c>
-      <c r="DD4">
+      <c r="DG4">
         <v>0.1195835845033234</v>
       </c>
-      <c r="DE4">
+      <c r="DH4">
         <v>-0.07668491299714397</v>
       </c>
-      <c r="DF4">
+      <c r="DI4">
         <v>1.09131066560171</v>
       </c>
-      <c r="DG4">
+      <c r="DJ4">
         <v>0.358639870563867</v>
       </c>
-      <c r="DH4">
+      <c r="DK4">
         <v>0.6755846507118362</v>
       </c>
-      <c r="DI4">
+      <c r="DL4">
         <v>0.05708614432600656</v>
       </c>
-      <c r="DJ4">
+      <c r="DM4">
         <v>0.8054368616610621</v>
       </c>
-      <c r="DK4">
+      <c r="DN4">
         <v>0.07276606662321938</v>
       </c>
-      <c r="DL4">
+      <c r="DO4">
         <v>0.1416944472884999</v>
       </c>
-      <c r="DM4">
+      <c r="DP4">
         <v>0.04214947113973488</v>
       </c>
-      <c r="DN4">
+      <c r="DQ4">
         <v>0.1296964554860001</v>
       </c>
-      <c r="DO4">
+      <c r="DR4">
         <v>0.03015147933723503</v>
       </c>
-      <c r="DP4">
+      <c r="DS4">
         <v>0.01504559783999614</v>
       </c>
-      <c r="DQ4">
+      <c r="DT4">
         <v>-0.07683906570901562</v>
       </c>
-      <c r="DR4">
-        <v>0</v>
-      </c>
-      <c r="DS4">
+      <c r="DU4">
+        <v>0</v>
+      </c>
+      <c r="DV4">
         <v>0.003244703005003044</v>
       </c>
-      <c r="DT4">
+      <c r="DW4">
         <v>0.03084997971804167</v>
       </c>
-      <c r="DU4">
+      <c r="DX4">
         <v>0.04081712638526287</v>
       </c>
-      <c r="DV4">
+      <c r="DY4">
         <v>0.01833154711700092</v>
       </c>
-      <c r="DW4">
+      <c r="DZ4">
         <v>0.0002466161494731993</v>
       </c>
-      <c r="DX4">
+      <c r="EA4">
         <v>0.0002466161494731993</v>
       </c>
     </row>
-    <row r="5" spans="1:128">
+    <row r="5" spans="1:131">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2535,157 +2580,166 @@
         <v>0.06216191645146874</v>
       </c>
       <c r="CA5">
+        <v>0.4454800764378618</v>
+      </c>
+      <c r="CB5">
+        <v>0.09067082488863261</v>
+      </c>
+      <c r="CC5">
+        <v>0.4638490986735056</v>
+      </c>
+      <c r="CD5">
         <v>4.019929437164723</v>
       </c>
-      <c r="CB5">
+      <c r="CE5">
         <v>0.4638490986735056</v>
       </c>
-      <c r="CC5">
+      <c r="CF5">
         <v>0.03985887432944387</v>
       </c>
-      <c r="CD5">
+      <c r="CG5">
         <v>0.1335239147345178</v>
       </c>
-      <c r="CE5">
+      <c r="CH5">
         <v>0.229889451799854</v>
       </c>
-      <c r="CF5">
+      <c r="CI5">
         <v>0.003909488002416688</v>
       </c>
-      <c r="CG5">
+      <c r="CJ5">
         <v>0.0863117182001216</v>
       </c>
-      <c r="CH5">
+      <c r="CK5">
         <v>0.8308809304636608</v>
       </c>
-      <c r="CI5">
+      <c r="CL5">
         <v>0.01633460109291129</v>
       </c>
-      <c r="CJ5">
-        <v>0</v>
-      </c>
-      <c r="CK5">
+      <c r="CM5">
+        <v>0</v>
+      </c>
+      <c r="CN5">
         <v>0.04582731535855744</v>
       </c>
-      <c r="CL5">
+      <c r="CO5">
         <v>0.0411970810024897</v>
       </c>
-      <c r="CM5">
+      <c r="CP5">
         <v>0.7960487865408556</v>
       </c>
-      <c r="CN5">
+      <c r="CQ5">
         <v>0.1145955081439621</v>
       </c>
-      <c r="CO5">
+      <c r="CR5">
         <v>0.7960487865408556</v>
       </c>
-      <c r="CP5">
+      <c r="CS5">
         <v>0.6588336283105337</v>
       </c>
-      <c r="CQ5">
+      <c r="CT5">
         <v>0.03985887432944387</v>
       </c>
-      <c r="CR5">
+      <c r="CU5">
         <v>0.1335239147345178</v>
       </c>
-      <c r="CS5">
+      <c r="CV5">
         <v>0.2251833779818854</v>
       </c>
-      <c r="CT5">
+      <c r="CW5">
         <v>0.1734160946631905</v>
       </c>
-      <c r="CU5">
+      <c r="CX5">
         <v>0.2251833779818854</v>
       </c>
-      <c r="CV5">
+      <c r="CY5">
         <v>1.523378094893009</v>
       </c>
-      <c r="CW5">
+      <c r="CZ5">
         <v>-4.105254582134899</v>
       </c>
-      <c r="CX5">
+      <c r="DA5">
         <v>-4.105254582134899</v>
       </c>
-      <c r="CY5">
+      <c r="DB5">
         <v>0.2635438530662409</v>
       </c>
-      <c r="CZ5">
+      <c r="DC5">
         <v>0.5252393507503761</v>
       </c>
-      <c r="DA5">
+      <c r="DD5">
         <v>0.5252393507503761</v>
       </c>
-      <c r="DB5">
+      <c r="DE5">
         <v>0.03836047508435547</v>
       </c>
-      <c r="DC5">
+      <c r="DF5">
         <v>0.2408578339134133</v>
       </c>
-      <c r="DD5">
+      <c r="DG5">
         <v>0.1086326222001996</v>
       </c>
-      <c r="DE5">
+      <c r="DH5">
         <v>0.01567445593152786</v>
       </c>
-      <c r="DF5">
+      <c r="DI5">
         <v>1.05582956340223</v>
       </c>
-      <c r="DG5">
+      <c r="DJ5">
         <v>0.2597807768613747</v>
       </c>
-      <c r="DH5">
+      <c r="DK5">
         <v>0.7031711309275829</v>
       </c>
-      <c r="DI5">
+      <c r="DL5">
         <v>0.09287765561327277</v>
       </c>
-      <c r="DJ5">
+      <c r="DM5">
         <v>0.7755075004580184</v>
       </c>
-      <c r="DK5">
+      <c r="DN5">
         <v>-0.02054128608283723</v>
       </c>
-      <c r="DL5">
+      <c r="DO5">
         <v>0.1042104921368445</v>
       </c>
-      <c r="DM5">
+      <c r="DP5">
         <v>-0.0103850160071176</v>
       </c>
-      <c r="DN5">
+      <c r="DQ5">
         <v>0.0912029845510345</v>
       </c>
-      <c r="DO5">
+      <c r="DR5">
         <v>-0.02339252359292764</v>
       </c>
-      <c r="DP5">
+      <c r="DS5">
         <v>0.01270632604870283</v>
       </c>
-      <c r="DQ5">
+      <c r="DT5">
         <v>-0.03312098930985462</v>
       </c>
-      <c r="DR5">
-        <v>0</v>
-      </c>
-      <c r="DS5">
+      <c r="DU5">
+        <v>0</v>
+      </c>
+      <c r="DV5">
         <v>0.003909488002416688</v>
       </c>
-      <c r="DT5">
+      <c r="DW5">
         <v>0.05390241064613877</v>
       </c>
-      <c r="DU5">
+      <c r="DX5">
         <v>0.01270532964364907</v>
       </c>
-      <c r="DV5">
+      <c r="DY5">
         <v>0.01933263694699735</v>
       </c>
-      <c r="DW5">
+      <c r="DZ5">
         <v>0.002998035854086058</v>
       </c>
-      <c r="DX5">
+      <c r="EA5">
         <v>0.002998035854086058</v>
       </c>
     </row>
-    <row r="6" spans="1:128">
+    <row r="6" spans="1:131">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2921,153 +2975,162 @@
         <v>0.06532529280368227</v>
       </c>
       <c r="CA6">
+        <v>0.4160467828935779</v>
+      </c>
+      <c r="CB6">
+        <v>0.1188040098591713</v>
+      </c>
+      <c r="CC6">
+        <v>0.4651492072472509</v>
+      </c>
+      <c r="CD6">
         <v>4.019069047212044</v>
       </c>
-      <c r="CB6">
+      <c r="CE6">
         <v>0.4651492072472509</v>
       </c>
-      <c r="CC6">
+      <c r="CF6">
         <v>0.03813809442408737</v>
       </c>
-      <c r="CD6">
+      <c r="CG6">
         <v>0.188429345968803</v>
       </c>
-      <c r="CE6">
+      <c r="CH6">
         <v>0.1683299875655219</v>
       </c>
-      <c r="CF6">
+      <c r="CI6">
         <v>0.001314929897532676</v>
       </c>
-      <c r="CG6">
+      <c r="CJ6">
         <v>0.08140682210975503</v>
       </c>
-      <c r="CH6">
+      <c r="CK6">
         <v>0.7778687091392527</v>
       </c>
-      <c r="CI6">
+      <c r="CL6">
         <v>0.02221500221701144</v>
       </c>
-      <c r="CJ6">
-        <v>0</v>
-      </c>
-      <c r="CK6">
+      <c r="CM6">
+        <v>0</v>
+      </c>
+      <c r="CN6">
         <v>0.04311029058667082</v>
       </c>
-      <c r="CL6">
+      <c r="CO6">
         <v>0.03595277320074403</v>
       </c>
-      <c r="CM6">
+      <c r="CP6">
         <v>0.8066936246191559</v>
       </c>
-      <c r="CN6">
+      <c r="CQ6">
         <v>0.1066518621869461</v>
       </c>
-      <c r="CO6">
+      <c r="CR6">
         <v>0.8066936246191559</v>
       </c>
-      <c r="CP6">
+      <c r="CS6">
         <v>0.6236780134539113</v>
       </c>
-      <c r="CQ6">
+      <c r="CT6">
         <v>0.03813809442408737</v>
       </c>
-      <c r="CR6">
+      <c r="CU6">
         <v>0.188429345968803</v>
       </c>
-      <c r="CS6">
+      <c r="CV6">
         <v>0.2233489229024943</v>
       </c>
-      <c r="CT6">
+      <c r="CW6">
         <v>0.1857526014875447</v>
       </c>
-      <c r="CU6">
+      <c r="CX6">
         <v>0.2233489229024943</v>
       </c>
-      <c r="CV6">
+      <c r="CY6">
         <v>1.310695653978269</v>
       </c>
-      <c r="CW6">
+      <c r="CZ6">
         <v>-5.018290049490754</v>
       </c>
-      <c r="CX6">
+      <c r="DA6">
         <v>-5.018290049490754</v>
       </c>
-      <c r="CY6">
+      <c r="DB6">
         <v>0.253683579899901</v>
       </c>
-      <c r="CZ6">
+      <c r="DC6">
         <v>0.4388745461934804</v>
       </c>
-      <c r="DA6">
+      <c r="DD6">
         <v>0.4388745461934804</v>
       </c>
-      <c r="DB6">
+      <c r="DE6">
         <v>0.0303346569974067</v>
       </c>
-      <c r="DC6">
+      <c r="DF6">
         <v>0.2278558410643445</v>
       </c>
-      <c r="DD6">
+      <c r="DG6">
         <v>0.1102635921495497</v>
       </c>
-      <c r="DE6">
+      <c r="DH6">
         <v>0.004506918161850199</v>
       </c>
-      <c r="DF6">
+      <c r="DI6">
         <v>1.10690166069113</v>
       </c>
-      <c r="DG6">
+      <c r="DJ6">
         <v>0.3002080360719742</v>
       </c>
-      <c r="DH6">
+      <c r="DK6">
         <v>0.7696181512387914</v>
       </c>
-      <c r="DI6">
+      <c r="DL6">
         <v>0.03707547338036454</v>
       </c>
-      <c r="DJ6">
+      <c r="DM6">
         <v>0.8005114743994316</v>
       </c>
-      <c r="DK6">
+      <c r="DN6">
         <v>-0.006182150219724347</v>
       </c>
-      <c r="DL6">
+      <c r="DO6">
         <v>0.07102254907238145</v>
       </c>
-      <c r="DM6">
+      <c r="DP6">
         <v>-0.0356293131145646</v>
       </c>
-      <c r="DN6">
+      <c r="DQ6">
         <v>0.07619903013648092</v>
       </c>
-      <c r="DO6">
+      <c r="DR6">
         <v>-0.03045283205046513</v>
       </c>
-      <c r="DP6">
+      <c r="DS6">
         <v>0.009733218967184942</v>
       </c>
-      <c r="DQ6">
+      <c r="DT6">
         <v>-0.03337707161948587</v>
       </c>
-      <c r="DR6">
-        <v>0</v>
-      </c>
-      <c r="DS6">
+      <c r="DU6">
+        <v>0</v>
+      </c>
+      <c r="DV6">
         <v>0.001314929897532676</v>
       </c>
-      <c r="DT6">
+      <c r="DW6">
         <v>0.05372105888613194</v>
       </c>
-      <c r="DU6">
+      <c r="DX6">
         <v>0.01776828568538791</v>
       </c>
-      <c r="DV6">
+      <c r="DY6">
         <v>0.02795390024574189</v>
       </c>
-      <c r="DW6">
+      <c r="DZ6">
         <v>0.005738898028730448</v>
       </c>
-      <c r="DX6">
+      <c r="EA6">
         <v>0.005738898028730448</v>
       </c>
     </row>

</xml_diff>